<commit_message>
0.0.10.0      07/09/2015 Added date & boolean valdation + filters. [3]
converted data from XML file to YML.
</commit_message>
<xml_diff>
--- a/docs/SAPI-Reference-Data-v2-2_01-June-2015.xlsx
+++ b/docs/SAPI-Reference-Data-v2-2_01-June-2015.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="7425" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="7425" firstSheet="4" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="VersionHistory" sheetId="5" r:id="rId1"/>
@@ -5398,7 +5398,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -5425,7 +5425,7 @@
         <v>1374</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="29.25" thickBot="1">
+    <row r="2" spans="1:4" ht="26.25" thickBot="1">
       <c r="A2" s="55" t="s">
         <v>1033</v>
       </c>
@@ -5453,7 +5453,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="43.5" thickBot="1">
+    <row r="4" spans="1:4" ht="39" thickBot="1">
       <c r="A4" s="55" t="s">
         <v>1036</v>
       </c>
@@ -5481,7 +5481,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="29.25" thickBot="1">
+    <row r="6" spans="1:4" ht="26.25" thickBot="1">
       <c r="A6" s="55" t="s">
         <v>1039</v>
       </c>
@@ -5495,7 +5495,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="29.25" thickBot="1">
+    <row r="7" spans="1:4" ht="26.25" thickBot="1">
       <c r="A7" s="55" t="s">
         <v>1041</v>
       </c>
@@ -5509,7 +5509,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" thickBot="1">
+    <row r="8" spans="1:4" ht="26.25" thickBot="1">
       <c r="A8" s="55" t="s">
         <v>1043</v>
       </c>
@@ -5523,7 +5523,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="29.25" thickBot="1">
+    <row r="9" spans="1:4" ht="26.25" thickBot="1">
       <c r="A9" s="55" t="s">
         <v>1045</v>
       </c>
@@ -5537,7 +5537,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" thickBot="1">
+    <row r="10" spans="1:4" ht="13.5" thickBot="1">
       <c r="A10" s="55" t="s">
         <v>1047</v>
       </c>
@@ -5551,7 +5551,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" thickBot="1">
+    <row r="11" spans="1:4" ht="26.25" thickBot="1">
       <c r="A11" s="55" t="s">
         <v>1049</v>
       </c>
@@ -5565,7 +5565,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" thickBot="1">
+    <row r="12" spans="1:4" ht="26.25" thickBot="1">
       <c r="A12" s="55" t="s">
         <v>1051</v>
       </c>
@@ -5579,7 +5579,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" thickBot="1">
+    <row r="13" spans="1:4" ht="26.25" thickBot="1">
       <c r="A13" s="55" t="s">
         <v>1053</v>
       </c>
@@ -5593,7 +5593,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" thickBot="1">
+    <row r="14" spans="1:4" ht="13.5" thickBot="1">
       <c r="A14" s="55" t="s">
         <v>1055</v>
       </c>
@@ -5607,7 +5607,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" thickBot="1">
+    <row r="15" spans="1:4" ht="13.5" thickBot="1">
       <c r="A15" s="55" t="s">
         <v>1057</v>
       </c>
@@ -5621,7 +5621,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="29.25" thickBot="1">
+    <row r="16" spans="1:4" ht="26.25" thickBot="1">
       <c r="A16" s="55" t="s">
         <v>1059</v>
       </c>
@@ -5635,7 +5635,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" thickBot="1">
+    <row r="17" spans="1:4" ht="13.5" thickBot="1">
       <c r="A17" s="55" t="s">
         <v>1061</v>
       </c>
@@ -5649,7 +5649,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="29.25" thickBot="1">
+    <row r="18" spans="1:4" ht="26.25" thickBot="1">
       <c r="A18" s="55" t="s">
         <v>1063</v>
       </c>
@@ -5663,7 +5663,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="29.25" thickBot="1">
+    <row r="19" spans="1:4" ht="26.25" thickBot="1">
       <c r="A19" s="55" t="s">
         <v>1065</v>
       </c>
@@ -5677,7 +5677,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="29.25" thickBot="1">
+    <row r="20" spans="1:4" ht="26.25" thickBot="1">
       <c r="A20" s="55" t="s">
         <v>1067</v>
       </c>
@@ -5691,7 +5691,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="29.25" thickBot="1">
+    <row r="21" spans="1:4" ht="26.25" thickBot="1">
       <c r="A21" s="55" t="s">
         <v>1069</v>
       </c>
@@ -5705,7 +5705,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="29.25" thickBot="1">
+    <row r="22" spans="1:4" ht="26.25" thickBot="1">
       <c r="A22" s="78" t="s">
         <v>1071</v>
       </c>
@@ -5719,7 +5719,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" thickBot="1">
+    <row r="23" spans="1:4" ht="13.5" thickBot="1">
       <c r="A23" s="55" t="s">
         <v>1072</v>
       </c>
@@ -5729,7 +5729,7 @@
         <v>1346</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="29.25" thickBot="1">
+    <row r="24" spans="1:4" ht="26.25" thickBot="1">
       <c r="A24" s="55" t="s">
         <v>1073</v>
       </c>
@@ -5757,7 +5757,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="29.25" thickBot="1">
+    <row r="26" spans="1:4" ht="26.25" thickBot="1">
       <c r="A26" s="55" t="s">
         <v>1076</v>
       </c>
@@ -5771,7 +5771,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="29.25" thickBot="1">
+    <row r="27" spans="1:4" ht="39" thickBot="1">
       <c r="A27" s="55" t="s">
         <v>1078</v>
       </c>
@@ -5785,7 +5785,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="28" spans="1:4" s="85" customFormat="1" ht="43.5" thickBot="1">
+    <row r="28" spans="1:4" s="85" customFormat="1" ht="39" thickBot="1">
       <c r="A28" s="78" t="s">
         <v>1129</v>
       </c>
@@ -5799,7 +5799,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="29" spans="1:4" s="85" customFormat="1" ht="29.25" thickBot="1">
+    <row r="29" spans="1:4" s="85" customFormat="1" ht="26.25" thickBot="1">
       <c r="A29" s="78" t="s">
         <v>1130</v>
       </c>
@@ -5813,7 +5813,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="30" spans="1:4" s="85" customFormat="1" ht="15" thickBot="1">
+    <row r="30" spans="1:4" s="85" customFormat="1" ht="13.5" thickBot="1">
       <c r="A30" s="78" t="s">
         <v>1131</v>
       </c>
@@ -5827,7 +5827,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="31" spans="1:4" s="85" customFormat="1" ht="29.25" thickBot="1">
+    <row r="31" spans="1:4" s="85" customFormat="1" ht="26.25" thickBot="1">
       <c r="A31" s="78" t="s">
         <v>1132</v>
       </c>
@@ -5841,7 +5841,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="32" spans="1:4" s="85" customFormat="1" ht="15" thickBot="1">
+    <row r="32" spans="1:4" s="85" customFormat="1" ht="26.25" thickBot="1">
       <c r="A32" s="78" t="s">
         <v>1133</v>
       </c>
@@ -5855,7 +5855,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="33" spans="1:4" s="85" customFormat="1" ht="29.25" thickBot="1">
+    <row r="33" spans="1:4" s="85" customFormat="1" ht="26.25" thickBot="1">
       <c r="A33" s="78" t="s">
         <v>1134</v>
       </c>
@@ -5869,7 +5869,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="34" spans="1:4" s="85" customFormat="1" ht="29.25" thickBot="1">
+    <row r="34" spans="1:4" s="85" customFormat="1" ht="26.25" thickBot="1">
       <c r="A34" s="78" t="s">
         <v>1135</v>
       </c>
@@ -5935,7 +5935,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="29.25" thickBot="1">
+    <row r="3" spans="1:6" ht="26.25" thickBot="1">
       <c r="A3" s="6" t="s">
         <v>927</v>
       </c>
@@ -5955,7 +5955,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" thickBot="1">
+    <row r="4" spans="1:6" ht="26.25" thickBot="1">
       <c r="A4" s="6" t="s">
         <v>927</v>
       </c>
@@ -5975,7 +5975,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="43.5" thickBot="1">
+    <row r="5" spans="1:6" ht="64.5" thickBot="1">
       <c r="A5" s="6" t="s">
         <v>927</v>
       </c>
@@ -5995,7 +5995,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="29.25" thickBot="1">
+    <row r="6" spans="1:6" ht="26.25" thickBot="1">
       <c r="A6" s="6" t="s">
         <v>937</v>
       </c>
@@ -6015,7 +6015,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="29.25" thickBot="1">
+    <row r="7" spans="1:6" ht="26.25" thickBot="1">
       <c r="A7" s="6" t="s">
         <v>927</v>
       </c>
@@ -6035,7 +6035,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="71.25">
+    <row r="8" spans="1:6" ht="63.75">
       <c r="A8" s="9" t="s">
         <v>927</v>
       </c>
@@ -6084,7 +6084,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6173,7 +6173,7 @@
   <dimension ref="A1:L323"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F1" sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
@@ -11198,7 +11198,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
@@ -11441,7 +11441,7 @@
   <dimension ref="A1:C113"/>
   <sheetViews>
     <sheetView topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
+      <selection activeCell="A93" sqref="A93:B113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12378,7 +12378,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12565,7 +12565,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12648,6 +12648,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -12655,9 +12656,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12780,6 +12781,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -12788,8 +12790,8 @@
   <dimension ref="A1:B265"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:B1"/>
+      <pane ySplit="1" topLeftCell="A264" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:B265"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14920,6 +14922,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -14927,16 +14930,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F135"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A106" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A116" sqref="A116:XFD117"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:B120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="73.5703125" style="54" customWidth="1"/>
-    <col min="3" max="3" width="67.140625" style="77" customWidth="1"/>
+    <col min="2" max="2" width="125.5703125" style="54" customWidth="1"/>
+    <col min="3" max="3" width="88.28515625" style="77" customWidth="1"/>
     <col min="4" max="4" width="65.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" customWidth="1"/>
   </cols>
@@ -14958,7 +14961,7 @@
         <v>1374</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="26" customFormat="1" ht="29.25" thickBot="1">
+    <row r="2" spans="1:6" s="26" customFormat="1" ht="26.25" thickBot="1">
       <c r="A2" s="90" t="s">
         <v>809</v>
       </c>
@@ -15132,7 +15135,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="26" customFormat="1" ht="29.25" thickBot="1">
+    <row r="13" spans="1:6" s="26" customFormat="1" ht="26.25" thickBot="1">
       <c r="A13" s="90" t="s">
         <v>829</v>
       </c>
@@ -15162,7 +15165,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="26" customFormat="1" ht="29.25" thickBot="1">
+    <row r="15" spans="1:6" s="26" customFormat="1" ht="26.25" thickBot="1">
       <c r="A15" s="90" t="s">
         <v>833</v>
       </c>
@@ -15177,7 +15180,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="26" customFormat="1" ht="29.25" thickBot="1">
+    <row r="16" spans="1:6" s="26" customFormat="1" ht="26.25" thickBot="1">
       <c r="A16" s="90" t="s">
         <v>835</v>
       </c>
@@ -15327,7 +15330,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="26" customFormat="1" ht="29.25" thickBot="1">
+    <row r="26" spans="1:5" s="26" customFormat="1" ht="26.25" thickBot="1">
       <c r="A26" s="90" t="s">
         <v>854</v>
       </c>
@@ -15342,7 +15345,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="26" customFormat="1" ht="15.75" thickBot="1">
+    <row r="27" spans="1:5" s="26" customFormat="1" ht="26.25" thickBot="1">
       <c r="A27" s="90" t="s">
         <v>856</v>
       </c>
@@ -15357,7 +15360,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="26" customFormat="1" ht="29.25" thickBot="1">
+    <row r="28" spans="1:5" s="26" customFormat="1" ht="26.25" thickBot="1">
       <c r="A28" s="90" t="s">
         <v>858</v>
       </c>
@@ -15417,7 +15420,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="26" customFormat="1" ht="29.25" thickBot="1">
+    <row r="32" spans="1:5" s="26" customFormat="1" ht="26.25" thickBot="1">
       <c r="A32" s="90" t="s">
         <v>865</v>
       </c>
@@ -15432,7 +15435,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="26" customFormat="1" ht="29.25" thickBot="1">
+    <row r="33" spans="1:5" s="26" customFormat="1" ht="39" thickBot="1">
       <c r="A33" s="90" t="s">
         <v>867</v>
       </c>
@@ -15447,7 +15450,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="26" customFormat="1" ht="29.25" thickBot="1">
+    <row r="34" spans="1:5" s="26" customFormat="1" ht="26.25" thickBot="1">
       <c r="A34" s="90" t="s">
         <v>868</v>
       </c>
@@ -15462,7 +15465,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="26" customFormat="1" ht="43.5" thickBot="1">
+    <row r="35" spans="1:5" s="26" customFormat="1" ht="39" thickBot="1">
       <c r="A35" s="90" t="s">
         <v>869</v>
       </c>
@@ -15477,7 +15480,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="26" customFormat="1" ht="43.5" thickBot="1">
+    <row r="36" spans="1:5" s="26" customFormat="1" ht="39" thickBot="1">
       <c r="A36" s="90" t="s">
         <v>870</v>
       </c>
@@ -15507,7 +15510,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="26" customFormat="1" ht="29.25" thickBot="1">
+    <row r="38" spans="1:5" s="26" customFormat="1" ht="26.25" thickBot="1">
       <c r="A38" s="90" t="s">
         <v>873</v>
       </c>
@@ -15732,7 +15735,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="26" customFormat="1" ht="271.5" thickBot="1">
+    <row r="53" spans="1:5" s="26" customFormat="1" ht="243" thickBot="1">
       <c r="A53" s="90" t="s">
         <v>900</v>
       </c>
@@ -15747,7 +15750,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="54" spans="1:5" s="26" customFormat="1" ht="300" thickBot="1">
+    <row r="54" spans="1:5" s="26" customFormat="1" ht="268.5" thickBot="1">
       <c r="A54" s="90" t="s">
         <v>902</v>
       </c>
@@ -15777,7 +15780,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="56" spans="1:5" s="26" customFormat="1" ht="29.25" thickBot="1">
+    <row r="56" spans="1:5" s="26" customFormat="1" ht="26.25" thickBot="1">
       <c r="A56" s="90" t="s">
         <v>906</v>
       </c>
@@ -15807,7 +15810,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="58" spans="1:5" s="26" customFormat="1" ht="29.25" thickBot="1">
+    <row r="58" spans="1:5" s="26" customFormat="1" ht="26.25" thickBot="1">
       <c r="A58" s="90" t="s">
         <v>908</v>
       </c>
@@ -15852,7 +15855,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="61" spans="1:5" s="26" customFormat="1" ht="29.25" thickBot="1">
+    <row r="61" spans="1:5" s="26" customFormat="1" ht="26.25" thickBot="1">
       <c r="A61" s="90" t="s">
         <v>911</v>
       </c>
@@ -15867,7 +15870,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="62" spans="1:5" s="26" customFormat="1" ht="29.25" thickBot="1">
+    <row r="62" spans="1:5" s="26" customFormat="1" ht="26.25" thickBot="1">
       <c r="A62" s="90" t="s">
         <v>912</v>
       </c>
@@ -15897,7 +15900,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="64" spans="1:5" s="26" customFormat="1" ht="29.25" thickBot="1">
+    <row r="64" spans="1:5" s="26" customFormat="1" ht="26.25" thickBot="1">
       <c r="A64" s="90" t="s">
         <v>914</v>
       </c>
@@ -15912,7 +15915,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="65" spans="1:5" s="26" customFormat="1" ht="29.25" thickBot="1">
+    <row r="65" spans="1:5" s="26" customFormat="1" ht="26.25" thickBot="1">
       <c r="A65" s="90" t="s">
         <v>916</v>
       </c>
@@ -15927,7 +15930,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="66" spans="1:5" s="26" customFormat="1" ht="29.25" thickBot="1">
+    <row r="66" spans="1:5" s="26" customFormat="1" ht="26.25" thickBot="1">
       <c r="A66" s="90" t="s">
         <v>917</v>
       </c>
@@ -15942,7 +15945,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="67" spans="1:5" s="26" customFormat="1" ht="29.25" thickBot="1">
+    <row r="67" spans="1:5" s="26" customFormat="1" ht="26.25" thickBot="1">
       <c r="A67" s="90" t="s">
         <v>918</v>
       </c>
@@ -16011,7 +16014,7 @@
         <v>1370</v>
       </c>
     </row>
-    <row r="72" spans="1:5" s="26" customFormat="1" ht="29.25" thickBot="1">
+    <row r="72" spans="1:5" s="26" customFormat="1" ht="26.25" thickBot="1">
       <c r="A72" s="90" t="s">
         <v>1311</v>
       </c>
@@ -16041,7 +16044,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="74" spans="1:5" s="26" customFormat="1" ht="29.25" thickBot="1">
+    <row r="74" spans="1:5" s="26" customFormat="1" ht="26.25" thickBot="1">
       <c r="A74" s="90" t="s">
         <v>1325</v>
       </c>
@@ -16101,7 +16104,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="78" spans="1:5" s="26" customFormat="1" ht="29.25" thickBot="1">
+    <row r="78" spans="1:5" s="26" customFormat="1" ht="26.25" thickBot="1">
       <c r="A78" s="90" t="s">
         <v>1322</v>
       </c>
@@ -16146,7 +16149,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="81" spans="1:5" s="26" customFormat="1" ht="29.25" thickBot="1">
+    <row r="81" spans="1:5" s="26" customFormat="1" ht="26.25" thickBot="1">
       <c r="A81" s="90" t="s">
         <v>1203</v>
       </c>
@@ -16176,7 +16179,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="83" spans="1:5" s="26" customFormat="1" ht="29.25" thickBot="1">
+    <row r="83" spans="1:5" s="26" customFormat="1" ht="26.25" thickBot="1">
       <c r="A83" s="90" t="s">
         <v>1205</v>
       </c>
@@ -16382,7 +16385,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="97" spans="1:5" s="26" customFormat="1" ht="29.25" thickBot="1">
+    <row r="97" spans="1:5" s="26" customFormat="1" ht="26.25" thickBot="1">
       <c r="A97" s="90" t="s">
         <v>1273</v>
       </c>
@@ -16397,7 +16400,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="98" spans="1:5" s="26" customFormat="1" ht="29.25" thickBot="1">
+    <row r="98" spans="1:5" s="26" customFormat="1" ht="26.25" thickBot="1">
       <c r="A98" s="90" t="s">
         <v>1274</v>
       </c>
@@ -16442,7 +16445,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="101" spans="1:5" s="26" customFormat="1" ht="29.25" thickBot="1">
+    <row r="101" spans="1:5" s="26" customFormat="1" ht="26.25" thickBot="1">
       <c r="A101" s="89" t="s">
         <v>1299</v>
       </c>
@@ -16468,7 +16471,7 @@
         <v>1370</v>
       </c>
     </row>
-    <row r="103" spans="1:5" s="26" customFormat="1" ht="29.25" thickBot="1">
+    <row r="103" spans="1:5" s="26" customFormat="1" ht="26.25" thickBot="1">
       <c r="A103" s="90" t="s">
         <v>1200</v>
       </c>
@@ -16483,7 +16486,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="104" spans="1:5" s="26" customFormat="1" ht="29.25" thickBot="1">
+    <row r="104" spans="1:5" s="26" customFormat="1" ht="26.25" thickBot="1">
       <c r="A104" s="90" t="s">
         <v>1340</v>
       </c>
@@ -16558,7 +16561,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="109" spans="1:5" s="26" customFormat="1" ht="29.25" thickBot="1">
+    <row r="109" spans="1:5" s="26" customFormat="1" ht="26.25" thickBot="1">
       <c r="A109" s="90" t="s">
         <v>1149</v>
       </c>
@@ -16584,7 +16587,7 @@
         <v>1370</v>
       </c>
     </row>
-    <row r="111" spans="1:5" s="26" customFormat="1" ht="29.25" thickBot="1">
+    <row r="111" spans="1:5" s="26" customFormat="1" ht="26.25" thickBot="1">
       <c r="A111" s="90" t="s">
         <v>1284</v>
       </c>
@@ -16599,7 +16602,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="112" spans="1:5" s="26" customFormat="1" ht="29.25" thickBot="1">
+    <row r="112" spans="1:5" s="26" customFormat="1" ht="26.25" thickBot="1">
       <c r="A112" s="90" t="s">
         <v>1152</v>
       </c>
@@ -16614,7 +16617,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="113" spans="1:6" s="26" customFormat="1" ht="29.25" thickBot="1">
+    <row r="113" spans="1:6" s="26" customFormat="1" ht="26.25" thickBot="1">
       <c r="A113" s="90" t="s">
         <v>1151</v>
       </c>
@@ -16630,7 +16633,7 @@
       </c>
       <c r="F113" s="75"/>
     </row>
-    <row r="114" spans="1:6" s="26" customFormat="1" ht="29.25" thickBot="1">
+    <row r="114" spans="1:6" s="26" customFormat="1" ht="39" thickBot="1">
       <c r="A114" s="90" t="s">
         <v>1150</v>
       </c>
@@ -16684,7 +16687,7 @@
         <v>1370</v>
       </c>
     </row>
-    <row r="118" spans="1:6" s="26" customFormat="1" ht="15.75" thickBot="1">
+    <row r="118" spans="1:6" s="26" customFormat="1" ht="26.25" thickBot="1">
       <c r="A118" s="90" t="s">
         <v>1252</v>
       </c>

</xml_diff>